<commit_message>
moved BNC to center for better access to lower profile connectors
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/eagle/projects/AdapterBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8607492-7F71-364C-AA09-C26728466EBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591EBBB8-2D7C-EA4B-8ECC-0CC0636EEC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{DF1953F2-50AB-EE4A-8FD3-B90F3BE883E5}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A2:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="H4">
         <f>IF(B$18*B4&gt;=10,G4,F4)*(B$18*B4)</f>
-        <v>32.400000000000006</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -682,7 +682,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>27.400000000000002</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -709,7 +709,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>7.6</v>
+        <v>0.84</v>
       </c>
       <c r="J8" t="s">
         <v>12</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -832,7 +832,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>5.2</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>23.599999999999998</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>23.599999999999998</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>6.2</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,11 +948,11 @@
         <v>6</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f>SUM(H4:H16)</f>
-        <v>135.29999999999998</v>
+        <v>14.64</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
increased constant current feedback resistor
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/eagle/projects/AdapterBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C430F0-8E8A-6D4B-AF01-59EB1E97DEC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F77B10B-B33E-2843-AD57-00614F12FCCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24760" yWindow="-3020" windowWidth="28040" windowHeight="17440" xr2:uid="{DF1953F2-50AB-EE4A-8FD3-B90F3BE883E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{DF1953F2-50AB-EE4A-8FD3-B90F3BE883E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,18 +186,9 @@
     <t>LM334M/NOPB</t>
   </si>
   <si>
-    <t>3.3 Ohm 0603</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>RC1608F3R3CS</t>
-  </si>
-  <si>
-    <t>436677 - 62</t>
-  </si>
-  <si>
     <t>100 Ohm 0603</t>
   </si>
   <si>
@@ -226,6 +217,15 @@
   </si>
   <si>
     <t>1311468 - 62</t>
+  </si>
+  <si>
+    <t>36 Ohm 0603</t>
+  </si>
+  <si>
+    <t>RC1608F36R0CS</t>
+  </si>
+  <si>
+    <t>436455 - 62</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H24"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,19 +891,19 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>0.91</v>
@@ -1053,19 +1053,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F19">
         <v>0.02</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1092,7 +1092,7 @@
         <v>1585242</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>0.02</v>
@@ -1107,19 +1107,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F21">
         <v>0.2</v>

</xml_diff>

<commit_message>
added LED to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/eagle/projects/AdapterBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F77B10B-B33E-2843-AD57-00614F12FCCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B54B51-CD52-184B-B397-3C2168004449}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{DF1953F2-50AB-EE4A-8FD3-B90F3BE883E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>436455 - 62</t>
+  </si>
+  <si>
+    <t>Power LED</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L 53 LID </t>
+  </si>
+  <si>
+    <t>146005 - 62</t>
   </si>
 </sst>
 </file>
@@ -581,7 +593,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,9 +1145,30 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22">
+        <v>0.12998000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.11998</v>
+      </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.12998000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>